<commit_message>
DataDriven and Parallel Test
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/LoginData.xlsx
+++ b/src/test/resources/TestData/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\IdeaProjects\ContactList_BDD\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCF9868-F8DF-4B98-A45E-A91ABDD95FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC39855E-1764-4BB5-8558-9DEADA48AC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{CE2F05D6-ACF2-441D-9917-21113DF8F326}"/>
   </bookViews>
@@ -461,9 +461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9FD671-AF06-4195-ACF1-79B2AAB41C9D}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>